<commit_message>
Update with Robbie fix from US model
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/RACP/RPS Alternative Compliance Payment.xlsx
+++ b/InputData/ctrl-settings/RACP/RPS Alternative Compliance Payment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\RACP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40486EA8-A6B9-4E6F-AA87-67D8340A717A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B141EEC2-7E62-4A27-99FB-390DD77E5144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -507,8 +507,8 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <f>100/About!A11</f>
-        <v>118.02137686524911</v>
+        <f>ROUND(100/About!A11,0)</f>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPS 4.0 updates as of 3/15/2024
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/RACP/RPS Alternative Compliance Payment.xlsx
+++ b/InputData/ctrl-settings/RACP/RPS Alternative Compliance Payment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\RACP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ctrl-settings\RACP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B141EEC2-7E62-4A27-99FB-390DD77E5144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC31C321-4E91-4E2D-AF32-8F21809892A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,8 +507,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <f>ROUND(100/About!A11,0)</f>
-        <v>118</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RACP update and webapp data text updates
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/RACP/RPS Alternative Compliance Payment.xlsx
+++ b/InputData/ctrl-settings/RACP/RPS Alternative Compliance Payment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ctrl-settings\RACP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\EPS Models\EU EPS\InputData\ctrl-settings\RACP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEEFDAE-23E8-4364-8ADC-79049DE0D37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0BD7C1-26A9-4BD9-BED9-19C64F9AD7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
+    <workbookView xWindow="37560" yWindow="255" windowWidth="25140" windowHeight="14625" activeTab="1" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAF84CE-31BD-44F2-91E9-58D4BA5F9B1E}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -491,8 +491,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>180</v>
+        <v>999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>